<commit_message>
add regression test for configuration file validation
</commit_message>
<xml_diff>
--- a/tests/regression_data/kofskey1972a_benner_1.xlsx
+++ b/tests/regression_data/kofskey1972a_benner_1.xlsx
@@ -2263,7 +2263,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AQ2"/>
+  <dimension ref="A1:AR2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2464,20 +2464,25 @@
       </c>
       <c r="AN1" s="1" t="inlineStr">
         <is>
+          <t>solidity</t>
+        </is>
+      </c>
+      <c r="AO1" s="1" t="inlineStr">
+        <is>
           <t>thickness_max_chord_ratio</t>
         </is>
       </c>
-      <c r="AO1" s="1" t="inlineStr">
+      <c r="AP1" s="1" t="inlineStr">
         <is>
           <t>thickness_te_opening_ratio</t>
         </is>
       </c>
-      <c r="AP1" s="1" t="inlineStr">
+      <c r="AQ1" s="1" t="inlineStr">
         <is>
           <t>tip_clearance_height_ratio</t>
         </is>
       </c>
-      <c r="AQ1" s="1" t="inlineStr">
+      <c r="AR1" s="1" t="inlineStr">
         <is>
           <t>diameter_le_chord_ratio</t>
         </is>
@@ -2679,20 +2684,25 @@
       </c>
       <c r="AN2" t="inlineStr">
         <is>
+          <t>[1.42997704 1.70997375]</t>
+        </is>
+      </c>
+      <c r="AO2" t="inlineStr">
+        <is>
           <t>[0.19304281 0.17152724]</t>
         </is>
       </c>
-      <c r="AO2" t="inlineStr">
+      <c r="AP2" t="inlineStr">
         <is>
           <t>[0.06467469 0.06897503]</t>
         </is>
       </c>
-      <c r="AP2" t="inlineStr">
+      <c r="AQ2" t="inlineStr">
         <is>
           <t>[0.         0.00820457]</t>
         </is>
       </c>
-      <c r="AQ2" t="inlineStr">
+      <c r="AR2" t="inlineStr">
         <is>
           <t>[0.0970948  0.06216424]</t>
         </is>

</xml_diff>